<commit_message>
Update results spreadsheet.  Modify MaxEnt script to use bigram features.
</commit_message>
<xml_diff>
--- a/output/results_summary.xlsx
+++ b/output/results_summary.xlsx
@@ -15,7 +15,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="21">
+  <si>
+    <t>features:</t>
+  </si>
+  <si>
+    <t>unigram presence</t>
+  </si>
+  <si>
+    <t>unigram presence, cut off of 4 (must occur at least 4 times)</t>
+  </si>
+  <si>
+    <t>note: with this feature set, the train accuracy is typically around 0.85 (corpuscine) and 0.95 (IMDB)</t>
+  </si>
+  <si>
+    <t>bigram presence</t>
+  </si>
   <si>
     <t>CorpusCine</t>
   </si>
@@ -75,6 +90,7 @@
   <fonts count="5">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -95,6 +111,7 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
@@ -142,9 +159,13 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
@@ -168,247 +189,562 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100">
-      <selection activeCell="D21" activeCellId="0" pane="topLeft" sqref="D21"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F39" activeCellId="0" pane="topLeft" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
-      <c r="A1" s="1" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
+      <c r="D1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>0.83</v>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0.825</v>
+        <v>0.83</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0.815</v>
+        <v>0.825</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.82</v>
+        <v>0.815</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.69</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0.86</v>
+        <v>0.82</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.605</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0.845</v>
+        <v>0.86</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.665</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>0.855</v>
+        <v>0.845</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.715</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.855</v>
       </c>
+      <c r="D9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0.815</v>
+        <v>0.855</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B11" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0.635</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="A12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="0" t="n">
         <v>0.82</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1" t="n">
-        <f aca="false">SUM(B2:B11)/10</f>
+      <c r="D12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0.715</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <f aca="false">SUM(B3:B12)/10</f>
         <v>0.834</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <f aca="false">MIN(B2:B11)</f>
+      <c r="D13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <f aca="false">SUM(E3:E12)/10</f>
+        <v>0.6745</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <f aca="false">SUM(H3:H12)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">MIN(B3:B12)</f>
         <v>0.815</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <f aca="false">MAX(B2:B11)</f>
+      <c r="D14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">MIN(E3:E12)</f>
+        <v>0.605</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">MIN(H3:H12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">MAX(B3:B12)</f>
         <v>0.86</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="D15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">MAX(E3:E12)</f>
+        <v>0.73</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">MAX(H3:H12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
-      <c r="A17" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>0.885</v>
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>0.88</v>
+        <v>0.885</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>0.82</v>
+        <v>0.88</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>0.81</v>
+        <v>0.82</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0.715</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>0.915</v>
+        <v>0.81</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>0.83</v>
+        <v>0.915</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0.705</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>0.855</v>
+        <v>0.83</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0.69</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>0.865</v>
+        <v>0.855</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>0.86</v>
+        <v>0.865</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B26" s="0" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0.645</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+      <c r="A27" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="0" t="n">
         <v>0.88</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
-      <c r="A27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="1" t="n">
-        <f aca="false">SUM(B17:B26)/10</f>
+      <c r="D27" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0.705</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <f aca="false">SUM(B18:B27)/10</f>
         <v>0.86</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
-      <c r="A28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="0" t="n">
-        <f aca="false">MIN(B17:B26)</f>
+      <c r="D28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <f aca="false">SUM(E18:E27)/10</f>
+        <v>0.682</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <f aca="false">SUM(H18:H27)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <f aca="false">MIN(B18:B27)</f>
         <v>0.81</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
-      <c r="A29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <f aca="false">MAX(B17:B26)</f>
+      <c r="D29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <f aca="false">MIN(E18:E27)</f>
+        <v>0.62</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <f aca="false">MIN(H18:H27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+      <c r="A30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <f aca="false">MAX(B18:B27)</f>
         <v>0.915</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <f aca="false">MAX(E18:E27)</f>
+        <v>0.715</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <f aca="false">MAX(H18:H27)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add results to results summary.
</commit_message>
<xml_diff>
--- a/output/results_summary.xlsx
+++ b/output/results_summary.xlsx
@@ -5,17 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="283" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="283" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="29">
   <si>
     <t>features:</t>
   </si>
@@ -35,6 +36,9 @@
     <t>trigram presence</t>
   </si>
   <si>
+    <t>unigram and bigram presence</t>
+  </si>
+  <si>
     <t>CorpusCine</t>
   </si>
   <si>
@@ -81,14 +85,33 @@
   </si>
   <si>
     <t>IMDB</t>
+  </si>
+  <si>
+    <t>features</t>
+  </si>
+  <si>
+    <t>unigram</t>
+  </si>
+  <si>
+    <t>unigram &gt; 4</t>
+  </si>
+  <si>
+    <t>bigram</t>
+  </si>
+  <si>
+    <t>trigram</t>
+  </si>
+  <si>
+    <t>unigram+bigram</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="0.00%" numFmtId="165"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -162,7 +185,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -173,6 +196,18 @@
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
@@ -192,10 +227,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="D1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="K6" activeCellId="0" pane="topLeft" sqref="K6"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="G1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="K28" activeCellId="0" pane="topLeft" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -236,698 +271,938 @@
       <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="M1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.83</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>0.73</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>0.835</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>0.825</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.825</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>0.65</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>0.81</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>0.81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.815</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>0.69</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>0.84</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>0.825</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.82</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0.605</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>0.78</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>0.795</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.86</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>0.665</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>0.835</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>0.84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.845</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>0.715</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>0.83</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>0.82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.855</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>0.67</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>0.855</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>0.865</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.855</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>0.67</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>0.87</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>0.865</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.815</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>0.635</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>0.815</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>0.795</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0.82</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0.715</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>0.84</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>0.83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2" t="n">
         <f aca="false">SUM(B3:B12)/10</f>
         <v>0.834</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E13" s="2" t="n">
         <f aca="false">SUM(E3:E12)/10</f>
         <v>0.6745</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H13" s="2" t="n">
         <f aca="false">SUM(H3:H12)/10</f>
         <v>0.831</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K13" s="2" t="n">
         <f aca="false">SUM(K3:K12)/10</f>
-        <v>0</v>
+        <v>0.818</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" s="2" t="n">
+        <f aca="false">SUM(N3:N12)/10</f>
+        <v>0.827</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="0" t="n">
         <f aca="false">MIN(B3:B12)</f>
         <v>0.815</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">MIN(E3:E12)</f>
         <v>0.605</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H14" s="0" t="n">
         <f aca="false">MIN(H3:H12)</f>
         <v>0.78</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K14" s="0" t="n">
         <f aca="false">MIN(K3:K12)</f>
-        <v>0</v>
+        <v>0.76</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <f aca="false">MIN(N3:N12)</f>
+        <v>0.795</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="0" t="n">
         <f aca="false">MAX(B3:B12)</f>
         <v>0.86</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E15" s="0" t="n">
         <f aca="false">MAX(E3:E12)</f>
         <v>0.73</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H15" s="0" t="n">
         <f aca="false">MAX(H3:H12)</f>
         <v>0.87</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K15" s="0" t="n">
         <f aca="false">MAX(K3:K12)</f>
-        <v>0</v>
+        <v>0.87</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <f aca="false">MAX(N3:N12)</f>
+        <v>0.865</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.885</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>0.7</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>0.855</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>0.87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.88</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>0.65</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>0.825</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>0.83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.82</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>0.715</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H20" s="0" t="n">
         <v>0.805</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M20" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>0.825</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.81</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>0.62</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>0.845</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>0.835</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0.915</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>0.705</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>0.88</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>0.89</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0.83</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>0.69</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H23" s="0" t="n">
         <v>0.855</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>0.845</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0.855</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>0.71</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H24" s="0" t="n">
         <v>0.85</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>0.495</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>0.855</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0.865</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>0.68</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H25" s="0" t="n">
         <v>0.86</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>0.87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0.86</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>0.645</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>0.835</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>0.505</v>
+      </c>
+      <c r="M26" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>0.855</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0.88</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>0.705</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H27" s="0" t="n">
         <v>0.855</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>0.495</v>
+      </c>
+      <c r="M27" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <v>0.86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B28" s="2" t="n">
         <f aca="false">SUM(B18:B27)/10</f>
         <v>0.86</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E28" s="2" t="n">
         <f aca="false">SUM(E18:E27)/10</f>
         <v>0.682</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H28" s="2" t="n">
         <f aca="false">SUM(H18:H27)/10</f>
         <v>0.8465</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K28" s="2" t="n">
         <f aca="false">SUM(K18:K27)/10</f>
-        <v>0</v>
+        <v>0.5005</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N28" s="2" t="n">
+        <f aca="false">SUM(N18:N27)/10</f>
+        <v>0.8535</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B29" s="0" t="n">
         <f aca="false">MIN(B18:B27)</f>
         <v>0.81</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E29" s="0" t="n">
         <f aca="false">MIN(E18:E27)</f>
         <v>0.62</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H29" s="0" t="n">
         <f aca="false">MIN(H18:H27)</f>
         <v>0.805</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K29" s="0" t="n">
         <f aca="false">MIN(K18:K27)</f>
-        <v>0</v>
+        <v>0.495</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N29" s="0" t="n">
+        <f aca="false">MIN(N18:N27)</f>
+        <v>0.825</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B30" s="0" t="n">
         <f aca="false">MAX(B18:B27)</f>
         <v>0.915</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E30" s="0" t="n">
         <f aca="false">MAX(E18:E27)</f>
         <v>0.715</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H30" s="0" t="n">
         <f aca="false">MAX(H18:H27)</f>
         <v>0.88</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K30" s="0" t="n">
         <f aca="false">MAX(K18:K27)</f>
-        <v>0</v>
+        <v>0.51</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N30" s="0" t="n">
+        <f aca="false">MAX(N18:N27)</f>
+        <v>0.89</v>
       </c>
     </row>
   </sheetData>
@@ -939,4 +1214,188 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C12" activeCellId="0" pane="topLeft" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.1"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="14.4897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>0.834</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>0.915</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
+      <c r="A4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>0.6745</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>0.605</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0.682</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>0.715</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>0.831</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>0.8465</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+      <c r="A6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>0.818</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0.5005</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0.495</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
+      <c r="A7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>0.827</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.865</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>0.8535</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add to results summary spreadsheet.
</commit_message>
<xml_diff>
--- a/output/results_summary.xlsx
+++ b/output/results_summary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="31">
   <si>
     <t>features:</t>
   </si>
@@ -39,6 +39,9 @@
     <t>unigram and bigram presence</t>
   </si>
   <si>
+    <t>unigrams from sentiment lexicon</t>
+  </si>
+  <si>
     <t>CorpusCine</t>
   </si>
   <si>
@@ -103,6 +106,9 @@
   </si>
   <si>
     <t>unigram+bigram</t>
+  </si>
+  <si>
+    <t>sentiment lexicon</t>
   </si>
 </sst>
 </file>
@@ -185,7 +191,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -199,6 +205,10 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -227,10 +237,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="G1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="K28" activeCellId="0" pane="topLeft" sqref="K28"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="H1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="L44" activeCellId="0" pane="topLeft" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -243,7 +253,7 @@
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="46.25" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -277,932 +287,1082 @@
       <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="P1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="K2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="N2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.83</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>0.73</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>0.835</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>0.84</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N3" s="0" t="n">
         <v>0.825</v>
       </c>
+      <c r="P3" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.825</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>0.65</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>0.81</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K4" s="0" t="n">
         <v>0.795</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N4" s="0" t="n">
         <v>0.81</v>
       </c>
+      <c r="P4" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.815</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>0.69</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>0.84</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>0.815</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>0.825</v>
       </c>
+      <c r="P5" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.82</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0.605</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>0.78</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>0.76</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N6" s="0" t="n">
         <v>0.795</v>
       </c>
+      <c r="P6" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.86</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>0.665</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>0.835</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K7" s="0" t="n">
         <v>0.815</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N7" s="0" t="n">
         <v>0.84</v>
       </c>
+      <c r="P7" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.845</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>0.715</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>0.83</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>0.815</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N8" s="0" t="n">
         <v>0.82</v>
       </c>
+      <c r="P8" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.855</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>0.67</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>0.855</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K9" s="0" t="n">
         <v>0.85</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N9" s="0" t="n">
         <v>0.865</v>
       </c>
+      <c r="P9" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.855</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>0.67</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>0.87</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K10" s="0" t="n">
         <v>0.87</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N10" s="0" t="n">
         <v>0.865</v>
       </c>
+      <c r="P10" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.815</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>0.635</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>0.815</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K11" s="0" t="n">
         <v>0.785</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N11" s="0" t="n">
         <v>0.795</v>
       </c>
+      <c r="P11" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0.82</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0.715</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>0.84</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>0.835</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N12" s="0" t="n">
         <v>0.83</v>
       </c>
+      <c r="P12" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2" t="n">
         <f aca="false">SUM(B3:B12)/10</f>
         <v>0.834</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E13" s="2" t="n">
         <f aca="false">SUM(E3:E12)/10</f>
         <v>0.6745</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H13" s="2" t="n">
         <f aca="false">SUM(H3:H12)/10</f>
         <v>0.831</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K13" s="2" t="n">
         <f aca="false">SUM(K3:K12)/10</f>
         <v>0.818</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N13" s="2" t="n">
         <f aca="false">SUM(N3:N12)/10</f>
         <v>0.827</v>
       </c>
+      <c r="P13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q13" s="2" t="n">
+        <f aca="false">SUM(Q3:Q12)/10</f>
+        <v>0</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="0" t="n">
         <f aca="false">MIN(B3:B12)</f>
         <v>0.815</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">MIN(E3:E12)</f>
         <v>0.605</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H14" s="0" t="n">
         <f aca="false">MIN(H3:H12)</f>
         <v>0.78</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K14" s="0" t="n">
         <f aca="false">MIN(K3:K12)</f>
         <v>0.76</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N14" s="0" t="n">
         <f aca="false">MIN(N3:N12)</f>
         <v>0.795</v>
       </c>
+      <c r="P14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <f aca="false">MIN(Q3:Q12)</f>
+        <v>0</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="0" t="n">
         <f aca="false">MAX(B3:B12)</f>
         <v>0.86</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E15" s="0" t="n">
         <f aca="false">MAX(E3:E12)</f>
         <v>0.73</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H15" s="0" t="n">
         <f aca="false">MAX(H3:H12)</f>
         <v>0.87</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K15" s="0" t="n">
         <f aca="false">MAX(K3:K12)</f>
         <v>0.87</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N15" s="0" t="n">
         <f aca="false">MAX(N3:N12)</f>
         <v>0.865</v>
       </c>
+      <c r="P15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <f aca="false">MAX(Q3:Q12)</f>
+        <v>0</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.885</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>0.7</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>0.855</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K18" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N18" s="0" t="n">
         <v>0.87</v>
       </c>
+      <c r="P18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>0.785</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.88</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>0.65</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>0.825</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K19" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N19" s="0" t="n">
         <v>0.83</v>
       </c>
+      <c r="P19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <v>0.81</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.82</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>0.715</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H20" s="0" t="n">
         <v>0.805</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K20" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N20" s="0" t="n">
         <v>0.825</v>
       </c>
+      <c r="P20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <v>0.755</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.81</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>0.62</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>0.845</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K21" s="0" t="n">
         <v>0.51</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N21" s="0" t="n">
         <v>0.835</v>
       </c>
+      <c r="P21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q21" s="0" t="n">
+        <v>0.74</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0.915</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>0.705</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>0.88</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K22" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N22" s="0" t="n">
         <v>0.89</v>
       </c>
+      <c r="P22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q22" s="0" t="n">
+        <v>0.805</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0.83</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>0.69</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H23" s="0" t="n">
         <v>0.855</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K23" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N23" s="0" t="n">
         <v>0.845</v>
       </c>
+      <c r="P23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q23" s="0" t="n">
+        <v>0.78</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0.855</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>0.71</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H24" s="0" t="n">
         <v>0.85</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K24" s="0" t="n">
         <v>0.495</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N24" s="0" t="n">
         <v>0.855</v>
       </c>
+      <c r="P24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q24" s="0" t="n">
+        <v>0.765</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0.865</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>0.68</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H25" s="0" t="n">
         <v>0.86</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K25" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N25" s="0" t="n">
         <v>0.87</v>
       </c>
+      <c r="P25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q25" s="0" t="n">
+        <v>0.83</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0.86</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>0.645</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>0.835</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K26" s="0" t="n">
         <v>0.505</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N26" s="0" t="n">
         <v>0.855</v>
       </c>
+      <c r="P26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q26" s="0" t="n">
+        <v>0.79</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0.88</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>0.705</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H27" s="0" t="n">
         <v>0.855</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K27" s="0" t="n">
         <v>0.495</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N27" s="0" t="n">
         <v>0.86</v>
       </c>
+      <c r="P27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q27" s="0" t="n">
+        <v>0.81</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B28" s="2" t="n">
         <f aca="false">SUM(B18:B27)/10</f>
         <v>0.86</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E28" s="2" t="n">
         <f aca="false">SUM(E18:E27)/10</f>
         <v>0.682</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H28" s="2" t="n">
         <f aca="false">SUM(H18:H27)/10</f>
         <v>0.8465</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K28" s="2" t="n">
         <f aca="false">SUM(K18:K27)/10</f>
         <v>0.5005</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N28" s="2" t="n">
         <f aca="false">SUM(N18:N27)/10</f>
         <v>0.8535</v>
       </c>
+      <c r="P28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q28" s="2" t="n">
+        <f aca="false">SUM(Q18:Q27)/10</f>
+        <v>0.787</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B29" s="0" t="n">
         <f aca="false">MIN(B18:B27)</f>
         <v>0.81</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E29" s="0" t="n">
         <f aca="false">MIN(E18:E27)</f>
         <v>0.62</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H29" s="0" t="n">
         <f aca="false">MIN(H18:H27)</f>
         <v>0.805</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K29" s="0" t="n">
         <f aca="false">MIN(K18:K27)</f>
         <v>0.495</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N29" s="0" t="n">
         <f aca="false">MIN(N18:N27)</f>
         <v>0.825</v>
       </c>
+      <c r="P29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q29" s="0" t="n">
+        <f aca="false">MIN(Q18:Q27)</f>
+        <v>0.74</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B30" s="0" t="n">
         <f aca="false">MAX(B18:B27)</f>
         <v>0.915</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E30" s="0" t="n">
         <f aca="false">MAX(E18:E27)</f>
         <v>0.715</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H30" s="0" t="n">
         <f aca="false">MAX(H18:H27)</f>
         <v>0.88</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K30" s="0" t="n">
         <f aca="false">MAX(K18:K27)</f>
         <v>0.51</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N30" s="0" t="n">
         <f aca="false">MAX(N18:N27)</f>
         <v>0.89</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q30" s="0" t="n">
+        <f aca="false">MAX(Q18:Q27)</f>
+        <v>0.83</v>
       </c>
     </row>
   </sheetData>
@@ -1221,10 +1381,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C12" activeCellId="0" pane="topLeft" sqref="C12"/>
+      <selection activeCell="D14" activeCellId="0" pane="topLeft" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -1235,154 +1395,171 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
       <c r="A1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="D2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>21</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
       <c r="A3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <v>0.915</v>
+      </c>
+      <c r="E3" s="6" t="n">
         <v>0.834</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="F3" s="6" t="n">
         <v>0.815</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="G3" s="6" t="n">
         <v>0.86</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <v>0.81</v>
-      </c>
-      <c r="G3" s="5" t="n">
-        <v>0.915</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="A4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="5" t="n">
+        <v>26</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>0.682</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>0.715</v>
+      </c>
+      <c r="E4" s="6" t="n">
         <v>0.6745</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="F4" s="6" t="n">
         <v>0.605</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="G4" s="6" t="n">
         <v>0.73</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>0.682</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="G4" s="5" t="n">
-        <v>0.715</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
       <c r="A5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>0.8465</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="E5" s="6" t="n">
         <v>0.831</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="F5" s="6" t="n">
         <v>0.78</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="G5" s="6" t="n">
         <v>0.87</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>0.8465</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>0.805</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>0.88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>0.5005</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>0.495</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="E6" s="6" t="n">
         <v>0.818</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="F6" s="6" t="n">
         <v>0.76</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="G6" s="6" t="n">
         <v>0.87</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <v>0.5005</v>
-      </c>
-      <c r="F6" s="5" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="G6" s="5" t="n">
-        <v>0.51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
       <c r="A7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>0.8535</v>
+      </c>
+      <c r="C7" s="6" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="E7" s="6" t="n">
         <v>0.827</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="F7" s="6" t="n">
         <v>0.795</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="G7" s="6" t="n">
         <v>0.865</v>
       </c>
-      <c r="E7" s="5" t="n">
-        <v>0.8535</v>
-      </c>
-      <c r="F7" s="5" t="n">
-        <v>0.825</v>
-      </c>
-      <c r="G7" s="5" t="n">
-        <v>0.89</v>
-      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+      <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>0.787</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Add Naive Bayes results to result summary spreadsheet.
</commit_message>
<xml_diff>
--- a/output/results_summary.xlsx
+++ b/output/results_summary.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="283" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="283" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="MaxEnt" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Naive Bayes" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="summary" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="33">
   <si>
     <t>features:</t>
   </si>
@@ -90,6 +91,9 @@
     <t>IMDB</t>
   </si>
   <si>
+    <t>MaxEnt</t>
+  </si>
+  <si>
     <t>features</t>
   </si>
   <si>
@@ -109,6 +113,9 @@
   </si>
   <si>
     <t>sentiment lexicon</t>
+  </si>
+  <si>
+    <t>Naive Bayes</t>
   </si>
 </sst>
 </file>
@@ -208,11 +215,11 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -237,9 +244,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="H1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A8" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="L44" activeCellId="0" pane="topLeft" sqref="L44"/>
     </sheetView>
   </sheetViews>
@@ -1365,6 +1372,7 @@
         <v>0.83</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1381,15 +1389,1158 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:Q44"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A13" activeCellId="0" pane="topLeft" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="46.25" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.69</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.655</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.605</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.635</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.685</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+      <c r="A9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+      <c r="A10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0.635</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="A11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0.595</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="A12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.865</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0.695</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <f aca="false">SUM(B3:B12)/10</f>
+        <v>0.827</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <f aca="false">SUM(E3:E12)/10</f>
+        <v>0.6475</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <f aca="false">SUM(H3:H12)/10</f>
+        <v>0.818</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <f aca="false">SUM(K3:K12)/10</f>
+        <v>0.8155</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" s="2" t="n">
+        <f aca="false">SUM(N3:N12)/10</f>
+        <v>0.8185</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q13" s="2" t="n">
+        <f aca="false">SUM(Q3:Q12)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">MIN(B3:B12)</f>
+        <v>0.79</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">MIN(E3:E12)</f>
+        <v>0.595</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">MIN(H3:H12)</f>
+        <v>0.785</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <f aca="false">MIN(K3:K12)</f>
+        <v>0.785</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <f aca="false">MIN(N3:N12)</f>
+        <v>0.78</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <f aca="false">MIN(Q3:Q12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">MAX(B3:B12)</f>
+        <v>0.865</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">MAX(E3:E12)</f>
+        <v>0.695</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">MAX(H3:H12)</f>
+        <v>0.85</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <f aca="false">MAX(K3:K12)</f>
+        <v>0.85</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <f aca="false">MAX(N3:N12)</f>
+        <v>0.85</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <f aca="false">MAX(Q3:Q12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+      <c r="A18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0.695</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>0.805</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+      <c r="A19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="P19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+      <c r="A20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="M20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="P20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <v>0.755</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+      <c r="A21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0.635</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="P21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q21" s="0" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+      <c r="A22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0.705</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="P22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q22" s="0" t="n">
+        <v>0.805</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+      <c r="A23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0.69</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>0.745</v>
+      </c>
+      <c r="P23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q23" s="0" t="n">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+      <c r="A24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="P24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q24" s="0" t="n">
+        <v>0.775</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+      <c r="A25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="P25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q25" s="0" t="n">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+      <c r="A26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="M26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="P26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q26" s="0" t="n">
+        <v>0.825</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+      <c r="A27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0.745</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="M27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="P27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q27" s="0" t="n">
+        <v>0.825</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <f aca="false">SUM(B18:B27)/10</f>
+        <v>0.8165</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <f aca="false">SUM(E18:E27)/10</f>
+        <v>0.692</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <f aca="false">SUM(H18:H27)/10</f>
+        <v>0.8115</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="2" t="n">
+        <f aca="false">SUM(K18:K27)/10</f>
+        <v>0.8095</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N28" s="2" t="n">
+        <f aca="false">SUM(N18:N27)/10</f>
+        <v>0.8145</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q28" s="2" t="n">
+        <f aca="false">SUM(Q18:Q27)/10</f>
+        <v>0.785</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <f aca="false">MIN(B18:B27)</f>
+        <v>0.75</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <f aca="false">MIN(E18:E27)</f>
+        <v>0.625</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <f aca="false">MIN(H18:H27)</f>
+        <v>0.735</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <f aca="false">MIN(K18:K27)</f>
+        <v>0.73</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N29" s="0" t="n">
+        <f aca="false">MIN(N18:N27)</f>
+        <v>0.745</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q29" s="0" t="n">
+        <f aca="false">MIN(Q18:Q27)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+      <c r="A30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <f aca="false">MAX(B18:B27)</f>
+        <v>0.87</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <f aca="false">MAX(E18:E27)</f>
+        <v>0.745</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <f aca="false">MAX(H18:H27)</f>
+        <v>0.855</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <f aca="false">MAX(K18:K27)</f>
+        <v>0.86</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" s="0" t="n">
+        <f aca="false">MAX(N18:N27)</f>
+        <v>0.855</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q30" s="0" t="n">
+        <f aca="false">MAX(Q18:Q27)</f>
+        <v>0.825</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D14" activeCellId="0" pane="topLeft" sqref="D14"/>
+      <selection activeCell="H19" activeCellId="0" pane="topLeft" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="14.4897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="15.7397959183673"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -1397,59 +2548,47 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="4"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+      <c r="A2" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="B2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
-      <c r="A3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="6" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="C3" s="6" t="n">
-        <v>0.81</v>
-      </c>
-      <c r="D3" s="6" t="n">
-        <v>0.915</v>
-      </c>
-      <c r="E3" s="6" t="n">
-        <v>0.834</v>
-      </c>
-      <c r="F3" s="6" t="n">
-        <v>0.815</v>
-      </c>
-      <c r="G3" s="6" t="n">
-        <v>0.86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
@@ -1457,22 +2596,22 @@
         <v>26</v>
       </c>
       <c r="B4" s="6" t="n">
-        <v>0.682</v>
+        <v>0.86</v>
       </c>
       <c r="C4" s="6" t="n">
-        <v>0.62</v>
+        <v>0.81</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>0.715</v>
+        <v>0.915</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>0.6745</v>
+        <v>0.834</v>
       </c>
       <c r="F4" s="6" t="n">
-        <v>0.605</v>
+        <v>0.815</v>
       </c>
       <c r="G4" s="6" t="n">
-        <v>0.73</v>
+        <v>0.86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
@@ -1480,92 +2619,299 @@
         <v>27</v>
       </c>
       <c r="B5" s="6" t="n">
-        <v>0.8465</v>
+        <v>0.682</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>0.805</v>
+        <v>0.62</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>0.88</v>
+        <v>0.715</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>0.831</v>
+        <v>0.6745</v>
       </c>
       <c r="F5" s="6" t="n">
-        <v>0.78</v>
+        <v>0.605</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="6" t="n">
-        <v>0.5005</v>
+        <v>0.8465</v>
       </c>
       <c r="C6" s="6" t="n">
-        <v>0.495</v>
+        <v>0.805</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>0.51</v>
+        <v>0.88</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>0.818</v>
+        <v>0.831</v>
       </c>
       <c r="F6" s="6" t="n">
-        <v>0.76</v>
+        <v>0.78</v>
       </c>
       <c r="G6" s="6" t="n">
         <v>0.87</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="6" t="n">
-        <v>0.8535</v>
+        <v>0.5005</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>0.825</v>
+        <v>0.495</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>0.89</v>
+        <v>0.51</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>0.827</v>
+        <v>0.818</v>
       </c>
       <c r="F7" s="6" t="n">
-        <v>0.795</v>
+        <v>0.76</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v>0.865</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="8">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="6" t="n">
+        <v>0.8535</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>0.827</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>0.865</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+      <c r="A9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="6" t="n">
         <v>0.787</v>
       </c>
-      <c r="C8" s="6" t="n">
+      <c r="C9" s="6" t="n">
         <v>0.74</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D9" s="6" t="n">
         <v>0.83</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="13">
+      <c r="A13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="A14" s="5"/>
+      <c r="B14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="15">
+      <c r="A15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="6" t="n">
+        <v>0.8165</v>
+      </c>
+      <c r="C15" s="6" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D15" s="6" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>0.827</v>
+      </c>
+      <c r="F15" s="6" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="G15" s="6" t="n">
+        <v>0.865</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="16">
+      <c r="A16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="6" t="n">
+        <v>0.692</v>
+      </c>
+      <c r="C16" s="6" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="D16" s="6" t="n">
+        <v>0.745</v>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>0.6475</v>
+      </c>
+      <c r="F16" s="6" t="n">
+        <v>0.595</v>
+      </c>
+      <c r="G16" s="6" t="n">
+        <v>0.695</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="17">
+      <c r="A17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="6" t="n">
+        <v>0.8115</v>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="D17" s="6" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>0.818</v>
+      </c>
+      <c r="F17" s="6" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+      <c r="A18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="6" t="n">
+        <v>0.8095</v>
+      </c>
+      <c r="C18" s="6" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="D18" s="6" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>0.8155</v>
+      </c>
+      <c r="F18" s="6" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="G18" s="6" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="19">
+      <c r="A19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="6" t="n">
+        <v>0.8145</v>
+      </c>
+      <c r="C19" s="6" t="n">
+        <v>0.745</v>
+      </c>
+      <c r="D19" s="6" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="E19" s="6" t="n">
+        <v>0.8185</v>
+      </c>
+      <c r="F19" s="6" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="G19" s="6" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+      <c r="A20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="6" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="C20" s="6" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D20" s="6" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
+  <mergeCells count="8">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add MaxEnt cut-off results to spreadsheet.
</commit_message>
<xml_diff>
--- a/output/results_summary.xlsx
+++ b/output/results_summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="283" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="569" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="MaxEnt" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="41">
   <si>
     <t>features:</t>
   </si>
@@ -89,6 +89,30 @@
   </si>
   <si>
     <t>IMDB</t>
+  </si>
+  <si>
+    <t>unigram presence, cut off of 1 (must occur at least once in training data)</t>
+  </si>
+  <si>
+    <t>unigram presence, cut off of 4 (must occur at least 4 times in training data)</t>
+  </si>
+  <si>
+    <t>bigram presence, cut off of 1 (must occur at least once in training data)</t>
+  </si>
+  <si>
+    <t>bigram presence, cut off of 3 (must occur at least 3 times in training data)</t>
+  </si>
+  <si>
+    <t>bigram presence, cut off of 4 (must occur at least 4 times in training data)</t>
+  </si>
+  <si>
+    <t>trigram presence, cut off of 1 (must occur at least once in training data)</t>
+  </si>
+  <si>
+    <t>trigram presence, cut off of 2 (must occur at least 2 times in training data)</t>
+  </si>
+  <si>
+    <t>trigram presence, cut off of 3 (must occur at least 3 times in training data)</t>
   </si>
   <si>
     <t>MaxEnt</t>
@@ -215,11 +239,11 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -244,10 +268,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q44"/>
+  <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A8" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="L44" activeCellId="0" pane="topLeft" sqref="L44"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="L25" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="S55" activeCellId="0" pane="topLeft" sqref="S55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1372,7 +1396,1505 @@
         <v>0.83</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="79.85" outlineLevel="0" r="33">
+      <c r="A33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="W33" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="34">
+      <c r="A34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="W34" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+      <c r="A35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K35" s="0" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="M35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N35" s="0" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q35" s="0" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="S35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="T35" s="0" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="V35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="W35" s="0" t="n">
+        <v>0.775</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
+      <c r="A36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>0.865</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="M36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="N36" s="0" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="P36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q36" s="0" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="S36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="T36" s="0" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="V36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="W36" s="0" t="n">
+        <v>0.775</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
+      <c r="A37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="M37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N37" s="0" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="P37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q37" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="S37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T37" s="0" t="n">
+        <v>0.745</v>
+      </c>
+      <c r="V37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="W37" s="0" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
+      <c r="A38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K38" s="0" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="M38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N38" s="0" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="P38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q38" s="0" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="S38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="T38" s="0" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="V38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="W38" s="0" t="n">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
+      <c r="A39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="M39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N39" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="P39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q39" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="S39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="T39" s="0" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="V39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="W39" s="0" t="n">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
+      <c r="A40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="M40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N40" s="0" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="P40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q40" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="S40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="T40" s="0" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="V40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="W40" s="0" t="n">
+        <v>0.765</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
+      <c r="A41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="M41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N41" s="0" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="P41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q41" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="S41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="T41" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="V41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="W41" s="0" t="n">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
+      <c r="A42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>0.865</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="M42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="N42" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="P42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q42" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="S42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="T42" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="V42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="W42" s="0" t="n">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
+      <c r="A43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H43" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="M43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N43" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="P43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q43" s="0" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="S43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T43" s="0" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="V43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="W43" s="0" t="n">
+        <v>0.725</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
+      <c r="A44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="M44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="N44" s="0" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q44" s="0" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="S44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="T44" s="0" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="V44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="W44" s="0" t="n">
+        <v>0.7955</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
+      <c r="A45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <f aca="false">SUM(B35:B44)/10</f>
+        <v>0.838</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <f aca="false">SUM(E35:E44)/10</f>
+        <v>0.8285</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H45" s="2" t="n">
+        <f aca="false">SUM(H35:H44)/10</f>
+        <v>0.809</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K45" s="2" t="n">
+        <f aca="false">SUM(K35:K44)/10</f>
+        <v>0.797</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N45" s="2" t="n">
+        <f aca="false">SUM(N35:N44)/10</f>
+        <v>0.793</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q45" s="2" t="n">
+        <f aca="false">SUM(Q35:Q44)/10</f>
+        <v>0.7855</v>
+      </c>
+      <c r="S45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T45" s="2" t="n">
+        <f aca="false">SUM(T35:T44)/10</f>
+        <v>0.768</v>
+      </c>
+      <c r="V45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W45" s="2" t="n">
+        <f aca="false">SUM(W35:W44)/10</f>
+        <v>0.75655</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
+      <c r="A46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <f aca="false">MIN(B35:B44)</f>
+        <v>0.805</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <f aca="false">MIN(E35:E44)</f>
+        <v>0.785</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <f aca="false">MIN(H35:H44)</f>
+        <v>0.75</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K46" s="0" t="n">
+        <f aca="false">MIN(K35:K44)</f>
+        <v>0.74</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N46" s="0" t="n">
+        <f aca="false">MIN(N35:N44)</f>
+        <v>0.74</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q46" s="0" t="n">
+        <f aca="false">MIN(Q35:Q44)</f>
+        <v>0.725</v>
+      </c>
+      <c r="S46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T46" s="0" t="n">
+        <f aca="false">MIN(T35:T44)</f>
+        <v>0.725</v>
+      </c>
+      <c r="V46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W46" s="0" t="n">
+        <f aca="false">MIN(W35:W44)</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
+      <c r="A47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <f aca="false">MAX(B35:B44)</f>
+        <v>0.88</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <f aca="false">MAX(E35:E44)</f>
+        <v>0.865</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <f aca="false">MAX(H35:H44)</f>
+        <v>0.845</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K47" s="0" t="n">
+        <f aca="false">MAX(K35:K44)</f>
+        <v>0.855</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N47" s="0" t="n">
+        <f aca="false">MAX(N35:N44)</f>
+        <v>0.845</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q47" s="0" t="n">
+        <f aca="false">MAX(Q35:Q44)</f>
+        <v>0.83</v>
+      </c>
+      <c r="S47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T47" s="0" t="n">
+        <f aca="false">MAX(T35:T44)</f>
+        <v>0.82</v>
+      </c>
+      <c r="V47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W47" s="0" t="n">
+        <f aca="false">MAX(W35:W44)</f>
+        <v>0.7955</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
+      <c r="A49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="T49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="W49" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
+      <c r="A50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K50" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="M50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N50" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="P50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q50" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="T50" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="V50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="W50" s="0" t="n">
+        <v>0.765</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
+      <c r="A51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H51" s="0" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K51" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="M51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="N51" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="P51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q51" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="T51" s="0" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="V51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="W51" s="0" t="n">
+        <v>0.745</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
+      <c r="A52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="J52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="K52" s="0" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="M52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N52" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="P52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q52" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T52" s="0" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="V52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="W52" s="0" t="n">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
+      <c r="A53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="J53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K53" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="M53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N53" s="0" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="P53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q53" s="0" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="S53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="T53" s="0" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="V53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="W53" s="0" t="n">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
+      <c r="A54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>0.915</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="J54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K54" s="0" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="M54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N54" s="0" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="P54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q54" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="T54" s="0" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="V54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="W54" s="0" t="n">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
+      <c r="A55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="J55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K55" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="M55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N55" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="P55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q55" s="0" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="S55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="T55" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="V55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="W55" s="0" t="n">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
+      <c r="A56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H56" s="0" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="J56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K56" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="M56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N56" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="P56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q56" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="T56" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="V56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="W56" s="0" t="n">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
+      <c r="A57" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="J57" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K57" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M57" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="N57" s="0" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="P57" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q57" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S57" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="T57" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="V57" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="W57" s="0" t="n">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
+      <c r="A58" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="J58" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="M58" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N58" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="P58" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q58" s="0" t="n">
+        <v>0.505</v>
+      </c>
+      <c r="S58" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T58" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="V58" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="W58" s="0" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
+      <c r="A59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>0.885</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="G59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H59" s="0" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="J59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K59" s="0" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="M59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="N59" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="P59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q59" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="T59" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="V59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="W59" s="0" t="n">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
+      <c r="A60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" s="2" t="n">
+        <f aca="false">SUM(B50:B59)/10</f>
+        <v>0.863</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60" s="2" t="n">
+        <f aca="false">SUM(E50:E59)/10</f>
+        <v>0.8605</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H60" s="2" t="n">
+        <f aca="false">SUM(H50:H59)/10</f>
+        <v>0.835</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K60" s="2" t="n">
+        <f aca="false">SUM(K50:K59)/10</f>
+        <v>0.815</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N60" s="2" t="n">
+        <f aca="false">SUM(N50:N59)/10</f>
+        <v>0.8115</v>
+      </c>
+      <c r="P60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q60" s="2" t="n">
+        <f aca="false">SUM(Q50:Q59)/10</f>
+        <v>0.504</v>
+      </c>
+      <c r="S60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T60" s="2" t="n">
+        <f aca="false">SUM(T50:T59)/10</f>
+        <v>0.7795</v>
+      </c>
+      <c r="V60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W60" s="2" t="n">
+        <f aca="false">SUM(W50:W59)/10</f>
+        <v>0.762</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
+      <c r="A61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <f aca="false">MIN(B50:B59)</f>
+        <v>0.815</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <f aca="false">MIN(E50:E59)</f>
+        <v>0.82</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H61" s="0" t="n">
+        <f aca="false">MIN(H50:H59)</f>
+        <v>0.81</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K61" s="0" t="n">
+        <f aca="false">MIN(K50:K59)</f>
+        <v>0.78</v>
+      </c>
+      <c r="M61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N61" s="0" t="n">
+        <f aca="false">MIN(N50:N59)</f>
+        <v>0.785</v>
+      </c>
+      <c r="P61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q61" s="0" t="n">
+        <f aca="false">MIN(Q50:Q59)</f>
+        <v>0.5</v>
+      </c>
+      <c r="S61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T61" s="0" t="n">
+        <f aca="false">MIN(T50:T59)</f>
+        <v>0.725</v>
+      </c>
+      <c r="V61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W61" s="0" t="n">
+        <f aca="false">MIN(W50:W59)</f>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
+      <c r="A62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <f aca="false">MAX(B50:B59)</f>
+        <v>0.915</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <f aca="false">MAX(E50:E59)</f>
+        <v>0.9</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H62" s="0" t="n">
+        <f aca="false">MAX(H50:H59)</f>
+        <v>0.86</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K62" s="0" t="n">
+        <f aca="false">MAX(K50:K59)</f>
+        <v>0.85</v>
+      </c>
+      <c r="M62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N62" s="0" t="n">
+        <f aca="false">MAX(N50:N59)</f>
+        <v>0.86</v>
+      </c>
+      <c r="P62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q62" s="0" t="n">
+        <f aca="false">MAX(Q50:Q59)</f>
+        <v>0.525</v>
+      </c>
+      <c r="S62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T62" s="0" t="n">
+        <f aca="false">MAX(T50:T59)</f>
+        <v>0.81</v>
+      </c>
+      <c r="V62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W62" s="0" t="n">
+        <f aca="false">MAX(W50:W59)</f>
+        <v>0.79</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2519,7 +4041,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2534,7 +4056,7 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="H19" activeCellId="0" pane="topLeft" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -2546,7 +4068,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
       <c r="A1" s="4" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2556,44 +4078,44 @@
       <c r="G1" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
-      <c r="A2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>0.86</v>
@@ -2616,7 +4138,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>0.682</v>
@@ -2639,7 +4161,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>0.8465</v>
@@ -2662,7 +4184,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>0.5005</v>
@@ -2685,7 +4207,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="8">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B8" s="6" t="n">
         <v>0.8535</v>
@@ -2708,7 +4230,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B9" s="6" t="n">
         <v>0.787</v>
@@ -2725,7 +4247,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2735,44 +4257,44 @@
       <c r="G12" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="13">
-      <c r="A13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
-      <c r="A14" s="5"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="15">
       <c r="A15" s="3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>0.8165</v>
@@ -2795,7 +4317,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="16">
       <c r="A16" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B16" s="6" t="n">
         <v>0.692</v>
@@ -2818,7 +4340,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="17">
       <c r="A17" s="3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>0.8115</v>
@@ -2841,7 +4363,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B18" s="6" t="n">
         <v>0.8095</v>
@@ -2864,7 +4386,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="19">
       <c r="A19" s="3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B19" s="6" t="n">
         <v>0.8145</v>
@@ -2887,7 +4409,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B20" s="6" t="n">
         <v>0.785</v>

</xml_diff>

<commit_message>
Add Naive Bayes results to spreadsheet.
</commit_message>
<xml_diff>
--- a/output/results_summary.xlsx
+++ b/output/results_summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="569" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="569" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="MaxEnt" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="43">
   <si>
     <t>features:</t>
   </si>
@@ -121,10 +121,16 @@
     <t>features</t>
   </si>
   <si>
+    <t>n-gram</t>
+  </si>
+  <si>
+    <t>cut-off</t>
+  </si>
+  <si>
     <t>unigram</t>
   </si>
   <si>
-    <t>unigram &gt; 4</t>
+    <t>none</t>
   </si>
   <si>
     <t>bigram</t>
@@ -222,7 +228,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -241,6 +247,10 @@
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
@@ -270,8 +280,8 @@
   </sheetPr>
   <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="L25" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="S55" activeCellId="0" pane="topLeft" sqref="S55"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="P22" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A60" activeCellId="0" pane="topLeft" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2911,10 +2921,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q44"/>
+  <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A13" activeCellId="0" pane="topLeft" sqref="A13"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A31" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="W62" activeCellId="0" pane="topLeft" sqref="W62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4037,7 +4047,1505 @@
         <v>0.825</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="79.85" outlineLevel="0" r="33">
+      <c r="A33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="W33" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="34">
+      <c r="A34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="W34" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+      <c r="A35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K35" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="M35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N35" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="P35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q35" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="S35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="T35" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="V35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="W35" s="0" t="n">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
+      <c r="A36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="M36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="N36" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="P36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q36" s="0" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="S36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="T36" s="0" t="n">
+        <v>0.745</v>
+      </c>
+      <c r="V36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="W36" s="0" t="n">
+        <v>0.725</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
+      <c r="A37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="M37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N37" s="0" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="P37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q37" s="0" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="S37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T37" s="0" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="V37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="W37" s="0" t="n">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
+      <c r="A38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K38" s="0" t="n">
+        <v>0.745</v>
+      </c>
+      <c r="M38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N38" s="0" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="P38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q38" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="S38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="T38" s="0" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="V38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="W38" s="0" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
+      <c r="A39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="M39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N39" s="0" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="P39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q39" s="0" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="S39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="T39" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="V39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="W39" s="0" t="n">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
+      <c r="A40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="M40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N40" s="0" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q40" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="S40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="T40" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="V40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="W40" s="0" t="n">
+        <v>0.775</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
+      <c r="A41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="M41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N41" s="0" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="P41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q41" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="S41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="T41" s="0" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="V41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="W41" s="0" t="n">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
+      <c r="A42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="M42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="N42" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="P42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q42" s="0" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="S42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="T42" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="V42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="W42" s="0" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
+      <c r="A43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H43" s="0" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="M43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N43" s="0" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="P43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q43" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="S43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T43" s="0" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="V43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="W43" s="0" t="n">
+        <v>0.735</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
+      <c r="A44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="M44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="N44" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="P44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q44" s="0" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="S44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="T44" s="0" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="V44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="W44" s="0" t="n">
+        <v>0.775</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
+      <c r="A45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <f aca="false">SUM(B35:B44)/10</f>
+        <v>0.8245</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <f aca="false">SUM(E35:E44)/10</f>
+        <v>0.8215</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H45" s="2" t="n">
+        <f aca="false">SUM(H35:H44)/10</f>
+        <v>0.806</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K45" s="2" t="n">
+        <f aca="false">SUM(K35:K44)/10</f>
+        <v>0.8005</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N45" s="2" t="n">
+        <f aca="false">SUM(N35:N44)/10</f>
+        <v>0.7915</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q45" s="2" t="n">
+        <f aca="false">SUM(Q35:Q44)/10</f>
+        <v>0.789</v>
+      </c>
+      <c r="S45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T45" s="2" t="n">
+        <f aca="false">SUM(T35:T44)/10</f>
+        <v>0.78</v>
+      </c>
+      <c r="V45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W45" s="2" t="n">
+        <f aca="false">SUM(W35:W44)/10</f>
+        <v>0.775</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
+      <c r="A46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <f aca="false">MIN(B35:B44)</f>
+        <v>0.8</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <f aca="false">MIN(E35:E44)</f>
+        <v>0.78</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <f aca="false">MIN(H35:H44)</f>
+        <v>0.76</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K46" s="0" t="n">
+        <f aca="false">MIN(K35:K44)</f>
+        <v>0.745</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N46" s="0" t="n">
+        <f aca="false">MIN(N35:N44)</f>
+        <v>0.74</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q46" s="0" t="n">
+        <f aca="false">MIN(Q35:Q44)</f>
+        <v>0.75</v>
+      </c>
+      <c r="S46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T46" s="0" t="n">
+        <f aca="false">MIN(T35:T44)</f>
+        <v>0.735</v>
+      </c>
+      <c r="V46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W46" s="0" t="n">
+        <f aca="false">MIN(W35:W44)</f>
+        <v>0.725</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
+      <c r="A47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <f aca="false">MAX(B35:B44)</f>
+        <v>0.85</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <f aca="false">MAX(E35:E44)</f>
+        <v>0.87</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <f aca="false">MAX(H35:H44)</f>
+        <v>0.845</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K47" s="0" t="n">
+        <f aca="false">MAX(K35:K44)</f>
+        <v>0.845</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N47" s="0" t="n">
+        <f aca="false">MAX(N35:N44)</f>
+        <v>0.835</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q47" s="0" t="n">
+        <f aca="false">MAX(Q35:Q44)</f>
+        <v>0.82</v>
+      </c>
+      <c r="S47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T47" s="0" t="n">
+        <f aca="false">MAX(T35:T44)</f>
+        <v>0.8</v>
+      </c>
+      <c r="V47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W47" s="0" t="n">
+        <f aca="false">MAX(W35:W44)</f>
+        <v>0.81</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
+      <c r="A49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="T49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="W49" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
+      <c r="A50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>0.885</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K50" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="M50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N50" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="P50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q50" s="0" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="S50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="T50" s="0" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="V50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="W50" s="0" t="n">
+        <v>0.735</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
+      <c r="A51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H51" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K51" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="M51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="N51" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="P51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q51" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="S51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="T51" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="V51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="W51" s="0" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
+      <c r="A52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="J52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="K52" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="M52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N52" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="P52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q52" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="S52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T52" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="V52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="W52" s="0" t="n">
+        <v>0.785</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
+      <c r="A53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="J53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K53" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="M53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N53" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="P53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q53" s="0" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="S53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="T53" s="0" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="V53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="W53" s="0" t="n">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
+      <c r="A54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="J54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K54" s="0" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="M54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N54" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="P54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q54" s="0" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="S54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="T54" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="V54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="W54" s="0" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
+      <c r="A55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="J55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K55" s="0" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="M55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N55" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="P55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q55" s="0" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="S55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="T55" s="0" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="V55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="W55" s="0" t="n">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
+      <c r="A56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H56" s="0" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="J56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K56" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="M56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N56" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="P56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q56" s="0" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="S56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="T56" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="V56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="W56" s="0" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
+      <c r="A57" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="J57" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K57" s="0" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="M57" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="N57" s="0" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="P57" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q57" s="0" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="S57" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="T57" s="0" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="V57" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="W57" s="0" t="n">
+        <v>0.765</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
+      <c r="A58" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="J58" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="M58" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N58" s="0" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="P58" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q58" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="S58" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T58" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="V58" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="W58" s="0" t="n">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
+      <c r="A59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="G59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H59" s="0" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="J59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K59" s="0" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="M59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="N59" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="P59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q59" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="S59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="T59" s="0" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="V59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="W59" s="0" t="n">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
+      <c r="A60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" s="2" t="n">
+        <f aca="false">SUM(B50:B59)/10</f>
+        <v>0.8195</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60" s="2" t="n">
+        <f aca="false">SUM(E50:E59)/10</f>
+        <v>0.8215</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H60" s="2" t="n">
+        <f aca="false">SUM(H50:H59)/10</f>
+        <v>0.8035</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K60" s="2" t="n">
+        <f aca="false">SUM(K50:K59)/10</f>
+        <v>0.8105</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N60" s="2" t="n">
+        <f aca="false">SUM(N50:N59)/10</f>
+        <v>0.8115</v>
+      </c>
+      <c r="P60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q60" s="2" t="n">
+        <f aca="false">SUM(Q50:Q59)/10</f>
+        <v>0.7825</v>
+      </c>
+      <c r="S60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T60" s="2" t="n">
+        <f aca="false">SUM(T50:T59)/10</f>
+        <v>0.7805</v>
+      </c>
+      <c r="V60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W60" s="2" t="n">
+        <f aca="false">SUM(W50:W59)/10</f>
+        <v>0.7665</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
+      <c r="A61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <f aca="false">MIN(B50:B59)</f>
+        <v>0.76</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <f aca="false">MIN(E50:E59)</f>
+        <v>0.76</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H61" s="0" t="n">
+        <f aca="false">MIN(H50:H59)</f>
+        <v>0.755</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K61" s="0" t="n">
+        <f aca="false">MIN(K50:K59)</f>
+        <v>0.77</v>
+      </c>
+      <c r="M61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N61" s="0" t="n">
+        <f aca="false">MIN(N50:N59)</f>
+        <v>0.785</v>
+      </c>
+      <c r="P61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q61" s="0" t="n">
+        <f aca="false">MIN(Q50:Q59)</f>
+        <v>0.74</v>
+      </c>
+      <c r="S61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T61" s="0" t="n">
+        <f aca="false">MIN(T50:T59)</f>
+        <v>0.72</v>
+      </c>
+      <c r="V61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W61" s="0" t="n">
+        <f aca="false">MIN(W50:W59)</f>
+        <v>0.73</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
+      <c r="A62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <f aca="false">MAX(B50:B59)</f>
+        <v>0.875</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <f aca="false">MAX(E50:E59)</f>
+        <v>0.885</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H62" s="0" t="n">
+        <f aca="false">MAX(H50:H59)</f>
+        <v>0.84</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K62" s="0" t="n">
+        <f aca="false">MAX(K50:K59)</f>
+        <v>0.845</v>
+      </c>
+      <c r="M62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N62" s="0" t="n">
+        <f aca="false">MAX(N50:N59)</f>
+        <v>0.84</v>
+      </c>
+      <c r="P62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q62" s="0" t="n">
+        <f aca="false">MAX(Q50:Q59)</f>
+        <v>0.815</v>
+      </c>
+      <c r="S62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T62" s="0" t="n">
+        <f aca="false">MAX(T50:T59)</f>
+        <v>0.82</v>
+      </c>
+      <c r="V62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W62" s="0" t="n">
+        <f aca="false">MAX(W50:W59)</f>
+        <v>0.81</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -4054,16 +5562,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H19" activeCellId="0" pane="topLeft" sqref="H19"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G32" activeCellId="0" pane="topLeft" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -4076,364 +5585,730 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="4"/>
       <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="A4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="6" t="n">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="7" t="n">
         <v>0.86</v>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="D4" s="7" t="n">
         <v>0.81</v>
       </c>
-      <c r="D4" s="6" t="n">
+      <c r="E4" s="7" t="n">
         <v>0.915</v>
       </c>
-      <c r="E4" s="6" t="n">
+      <c r="F4" s="7" t="n">
         <v>0.834</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="G4" s="7" t="n">
         <v>0.815</v>
       </c>
-      <c r="G4" s="6" t="n">
+      <c r="H4" s="7" t="n">
         <v>0.86</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
-      <c r="A5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="6" t="n">
-        <v>0.682</v>
-      </c>
-      <c r="C5" s="6" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="D5" s="6" t="n">
-        <v>0.715</v>
-      </c>
-      <c r="E5" s="6" t="n">
-        <v>0.6745</v>
-      </c>
-      <c r="F5" s="6" t="n">
-        <v>0.605</v>
-      </c>
-      <c r="G5" s="6" t="n">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
-      <c r="A6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="6" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+      <c r="B5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>0.863</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>0.915</v>
+      </c>
+      <c r="F5" s="7" t="n">
+        <v>0.838</v>
+      </c>
+      <c r="G5" s="7" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+      <c r="B6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>0.8605</v>
+      </c>
+      <c r="D6" s="7" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="E6" s="7" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="F6" s="7" t="n">
+        <v>0.8285</v>
+      </c>
+      <c r="G6" s="7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0.845</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
+      <c r="A7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="7" t="n">
         <v>0.8465</v>
       </c>
-      <c r="C6" s="6" t="n">
+      <c r="D7" s="7" t="n">
         <v>0.805</v>
       </c>
-      <c r="D6" s="6" t="n">
+      <c r="E7" s="7" t="n">
         <v>0.88</v>
       </c>
-      <c r="E6" s="6" t="n">
+      <c r="F7" s="7" t="n">
         <v>0.831</v>
       </c>
-      <c r="F6" s="6" t="n">
+      <c r="G7" s="7" t="n">
         <v>0.78</v>
       </c>
-      <c r="G6" s="6" t="n">
+      <c r="H7" s="7" t="n">
         <v>0.87</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
-      <c r="A7" s="3" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+      <c r="B8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="F8" s="7" t="n">
+        <v>0.809</v>
+      </c>
+      <c r="G8" s="7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0.845</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+      <c r="B9" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="D9" s="7" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="E9" s="7" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="F9" s="7" t="n">
+        <v>0.797</v>
+      </c>
+      <c r="G9" s="7" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0.855</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+      <c r="B10" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>0.8115</v>
+      </c>
+      <c r="D10" s="7" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="E10" s="7" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="F10" s="7" t="n">
+        <v>0.793</v>
+      </c>
+      <c r="G10" s="7" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0.845</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="A11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="C11" s="7" t="n">
         <v>0.5005</v>
       </c>
-      <c r="C7" s="6" t="n">
+      <c r="D11" s="7" t="n">
         <v>0.495</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="E11" s="7" t="n">
         <v>0.51</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="F11" s="7" t="n">
         <v>0.818</v>
       </c>
-      <c r="F7" s="6" t="n">
+      <c r="G11" s="7" t="n">
         <v>0.76</v>
       </c>
-      <c r="G7" s="6" t="n">
+      <c r="H11" s="7" t="n">
         <v>0.87</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="8">
-      <c r="A8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="6" t="n">
-        <v>0.8535</v>
-      </c>
-      <c r="C8" s="6" t="n">
-        <v>0.825</v>
-      </c>
-      <c r="D8" s="6" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="E8" s="6" t="n">
-        <v>0.827</v>
-      </c>
-      <c r="F8" s="6" t="n">
-        <v>0.795</v>
-      </c>
-      <c r="G8" s="6" t="n">
-        <v>0.865</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
-      <c r="A9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="6" t="n">
-        <v>0.787</v>
-      </c>
-      <c r="C9" s="6" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="D9" s="6" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="B12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>0.504</v>
+      </c>
+      <c r="D12" s="7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="7" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="F12" s="7" t="n">
+        <v>0.7855</v>
+      </c>
+      <c r="G12" s="7" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="H12" s="7" t="n">
         <v>0.83</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
-      <c r="A12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="13">
-      <c r="A13" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+      <c r="B13" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>0.7795</v>
+      </c>
+      <c r="D13" s="7" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="E13" s="7" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="F13" s="7" t="n">
+        <v>0.768</v>
+      </c>
+      <c r="G13" s="7" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <v>0.82</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>22</v>
+      <c r="B14" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="7" t="n">
+        <v>0.762</v>
+      </c>
+      <c r="D14" s="7" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="E14" s="7" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="F14" s="7" t="n">
+        <v>0.75655</v>
+      </c>
+      <c r="G14" s="7" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H14" s="7" t="n">
+        <v>0.7955</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="15">
       <c r="A15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="7" t="n">
+        <v>0.8535</v>
+      </c>
+      <c r="D15" s="7" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="E15" s="7" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="F15" s="7" t="n">
+        <v>0.827</v>
+      </c>
+      <c r="G15" s="7" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <v>0.865</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+      <c r="A16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="7" t="n">
+        <v>0.787</v>
+      </c>
+      <c r="D16" s="7" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="E16" s="7" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+      <c r="A19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="20">
+      <c r="A20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+      <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="6" t="n">
+      <c r="B21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="22">
+      <c r="A22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="7" t="n">
         <v>0.8165</v>
       </c>
-      <c r="C15" s="6" t="n">
+      <c r="D22" s="7" t="n">
         <v>0.75</v>
       </c>
-      <c r="D15" s="6" t="n">
+      <c r="E22" s="7" t="n">
         <v>0.87</v>
       </c>
-      <c r="E15" s="6" t="n">
+      <c r="F22" s="7" t="n">
         <v>0.827</v>
       </c>
-      <c r="F15" s="6" t="n">
+      <c r="G22" s="7" t="n">
         <v>0.79</v>
       </c>
-      <c r="G15" s="6" t="n">
+      <c r="H22" s="7" t="n">
         <v>0.865</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="16">
-      <c r="A16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="6" t="n">
-        <v>0.692</v>
-      </c>
-      <c r="C16" s="6" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="D16" s="6" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+      <c r="B23" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="7" t="n">
+        <v>0.8195</v>
+      </c>
+      <c r="D23" s="7" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="E23" s="7" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="F23" s="7" t="n">
+        <v>0.8245</v>
+      </c>
+      <c r="G23" s="7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H23" s="7" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+      <c r="B24" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C24" s="7" t="n">
+        <v>0.8215</v>
+      </c>
+      <c r="D24" s="7" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="E24" s="7" t="n">
+        <v>0.885</v>
+      </c>
+      <c r="F24" s="7" t="n">
+        <v>0.8215</v>
+      </c>
+      <c r="G24" s="7" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="H24" s="7" t="n">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="25">
+      <c r="A25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="7" t="n">
+        <v>0.8115</v>
+      </c>
+      <c r="D25" s="7" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="E25" s="7" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="F25" s="7" t="n">
+        <v>0.818</v>
+      </c>
+      <c r="G25" s="7" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="H25" s="7" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+      <c r="B26" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="7" t="n">
+        <v>0.8035</v>
+      </c>
+      <c r="D26" s="7" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="E26" s="7" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="F26" s="7" t="n">
+        <v>0.806</v>
+      </c>
+      <c r="G26" s="7" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="H26" s="7" t="n">
+        <v>0.845</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+      <c r="B27" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C27" s="7" t="n">
+        <v>0.8105</v>
+      </c>
+      <c r="D27" s="7" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="E27" s="7" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="F27" s="7" t="n">
+        <v>0.8005</v>
+      </c>
+      <c r="G27" s="7" t="n">
         <v>0.745</v>
       </c>
-      <c r="E16" s="6" t="n">
-        <v>0.6475</v>
-      </c>
-      <c r="F16" s="6" t="n">
-        <v>0.595</v>
-      </c>
-      <c r="G16" s="6" t="n">
-        <v>0.695</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="17">
-      <c r="A17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="6" t="n">
+      <c r="H27" s="7" t="n">
+        <v>0.845</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+      <c r="B28" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C28" s="7" t="n">
         <v>0.8115</v>
       </c>
-      <c r="C17" s="6" t="n">
+      <c r="D28" s="7" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="E28" s="7" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="F28" s="7" t="n">
+        <v>0.7915</v>
+      </c>
+      <c r="G28" s="7" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="H28" s="7" t="n">
+        <v>0.835</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+      <c r="A29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="7" t="n">
+        <v>0.8095</v>
+      </c>
+      <c r="D29" s="7" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="E29" s="7" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="F29" s="7" t="n">
+        <v>0.8155</v>
+      </c>
+      <c r="G29" s="7" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="H29" s="7" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+      <c r="B30" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="7" t="n">
+        <v>0.7825</v>
+      </c>
+      <c r="D30" s="7" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="E30" s="7" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="F30" s="7" t="n">
+        <v>0.789</v>
+      </c>
+      <c r="G30" s="7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="H30" s="7" t="n">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+      <c r="B31" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C31" s="7" t="n">
+        <v>0.7805</v>
+      </c>
+      <c r="D31" s="7" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="E31" s="7" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="F31" s="7" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="G31" s="7" t="n">
         <v>0.735</v>
       </c>
-      <c r="D17" s="6" t="n">
+      <c r="H31" s="7" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+      <c r="B32" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C32" s="7" t="n">
+        <v>0.7665</v>
+      </c>
+      <c r="D32" s="7" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="E32" s="7" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="F32" s="7" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="G32" s="7" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="H32" s="7" t="n">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="33">
+      <c r="A33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="7" t="n">
+        <v>0.8145</v>
+      </c>
+      <c r="D33" s="7" t="n">
+        <v>0.745</v>
+      </c>
+      <c r="E33" s="7" t="n">
         <v>0.855</v>
       </c>
-      <c r="E17" s="6" t="n">
-        <v>0.818</v>
-      </c>
-      <c r="F17" s="6" t="n">
+      <c r="F33" s="7" t="n">
+        <v>0.8185</v>
+      </c>
+      <c r="G33" s="7" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="H33" s="7" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+      <c r="A34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="7" t="n">
         <v>0.785</v>
       </c>
-      <c r="G17" s="6" t="n">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
-      <c r="A18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="6" t="n">
-        <v>0.8095</v>
-      </c>
-      <c r="C18" s="6" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="D18" s="6" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="E18" s="6" t="n">
-        <v>0.8155</v>
-      </c>
-      <c r="F18" s="6" t="n">
-        <v>0.785</v>
-      </c>
-      <c r="G18" s="6" t="n">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="19">
-      <c r="A19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="6" t="n">
-        <v>0.8145</v>
-      </c>
-      <c r="C19" s="6" t="n">
-        <v>0.745</v>
-      </c>
-      <c r="D19" s="6" t="n">
-        <v>0.855</v>
-      </c>
-      <c r="E19" s="6" t="n">
-        <v>0.8185</v>
-      </c>
-      <c r="F19" s="6" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="G19" s="6" t="n">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
-      <c r="A20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="6" t="n">
-        <v>0.785</v>
-      </c>
-      <c r="C20" s="6" t="n">
+      <c r="D34" s="7" t="n">
         <v>0.75</v>
       </c>
-      <c r="D20" s="6" t="n">
+      <c r="E34" s="7" t="n">
         <v>0.825</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:H20"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add CorpusCine sentiment lexicon results to results spreadsheet.
</commit_message>
<xml_diff>
--- a/output/results_summary.xlsx
+++ b/output/results_summary.xlsx
@@ -40,7 +40,7 @@
     <t>unigram and bigram presence</t>
   </si>
   <si>
-    <t>unigrams from sentiment lexicon</t>
+    <t>unigrams from sentiment lexicon (translated for CorpusCine)</t>
   </si>
   <si>
     <t>CorpusCine</t>
@@ -280,8 +280,8 @@
   </sheetPr>
   <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="P22" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A60" activeCellId="0" pane="topLeft" sqref="A60"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="I1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="Q13" activeCellId="1" pane="topLeft" sqref="K10:K11 Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -291,7 +291,9 @@
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4489795918367"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="46.25" outlineLevel="0" r="1">
@@ -407,6 +409,9 @@
       <c r="P3" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="Q3" s="0" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
@@ -442,6 +447,9 @@
       <c r="P4" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="Q4" s="0" t="n">
+        <v>0.76</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
@@ -477,6 +485,9 @@
       <c r="P5" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="Q5" s="0" t="n">
+        <v>0.755</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
@@ -512,6 +523,9 @@
       <c r="P6" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="Q6" s="0" t="n">
+        <v>0.705</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
@@ -547,6 +561,9 @@
       <c r="P7" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="Q7" s="0" t="n">
+        <v>0.69</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
@@ -582,6 +599,9 @@
       <c r="P8" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="Q8" s="0" t="n">
+        <v>0.765</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
@@ -617,6 +637,9 @@
       <c r="P9" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="Q9" s="0" t="n">
+        <v>0.765</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
@@ -652,6 +675,9 @@
       <c r="P10" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="Q10" s="0" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
@@ -687,6 +713,9 @@
       <c r="P11" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="Q11" s="0" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
@@ -722,6 +751,9 @@
       <c r="P12" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="Q12" s="0" t="n">
+        <v>0.765</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="2" t="s">
@@ -764,7 +796,7 @@
       </c>
       <c r="Q13" s="2" t="n">
         <f aca="false">SUM(Q3:Q12)/10</f>
-        <v>0</v>
+        <v>0.7405</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
@@ -808,7 +840,7 @@
       </c>
       <c r="Q14" s="0" t="n">
         <f aca="false">MIN(Q3:Q12)</f>
-        <v>0</v>
+        <v>0.69</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
@@ -852,7 +884,7 @@
       </c>
       <c r="Q15" s="0" t="n">
         <f aca="false">MAX(Q3:Q12)</f>
-        <v>0</v>
+        <v>0.765</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16"/>
@@ -2923,8 +2955,8 @@
   </sheetPr>
   <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A31" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="W62" activeCellId="0" pane="topLeft" sqref="W62"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="J1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="Q13" activeCellId="1" pane="topLeft" sqref="K10:K11 Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2934,7 +2966,9 @@
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4489795918367"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.8877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="46.25" outlineLevel="0" r="1">
@@ -3048,6 +3082,9 @@
       <c r="P3" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="Q3" s="0" t="n">
+        <v>0.74</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
@@ -3083,6 +3120,9 @@
       <c r="P4" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="Q4" s="0" t="n">
+        <v>0.79</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
@@ -3118,6 +3158,9 @@
       <c r="P5" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="Q5" s="0" t="n">
+        <v>0.71</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
@@ -3153,6 +3196,9 @@
       <c r="P6" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="Q6" s="0" t="n">
+        <v>0.685</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
@@ -3188,6 +3234,9 @@
       <c r="P7" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="Q7" s="0" t="n">
+        <v>0.79</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
@@ -3223,6 +3272,9 @@
       <c r="P8" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="Q8" s="0" t="n">
+        <v>0.755</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
@@ -3258,6 +3310,9 @@
       <c r="P9" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="Q9" s="0" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
@@ -3293,6 +3348,9 @@
       <c r="P10" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="Q10" s="0" t="n">
+        <v>0.825</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
@@ -3328,6 +3386,9 @@
       <c r="P11" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="Q11" s="0" t="n">
+        <v>0.74</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
@@ -3363,6 +3424,9 @@
       <c r="P12" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="Q12" s="0" t="n">
+        <v>0.73</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="2" t="s">
@@ -3405,7 +3469,7 @@
       </c>
       <c r="Q13" s="2" t="n">
         <f aca="false">SUM(Q3:Q12)/10</f>
-        <v>0</v>
+        <v>0.7515</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
@@ -3449,7 +3513,7 @@
       </c>
       <c r="Q14" s="0" t="n">
         <f aca="false">MIN(Q3:Q12)</f>
-        <v>0</v>
+        <v>0.685</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
@@ -3493,7 +3557,7 @@
       </c>
       <c r="Q15" s="0" t="n">
         <f aca="false">MAX(Q3:Q12)</f>
-        <v>0</v>
+        <v>0.825</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16"/>
@@ -5565,7 +5629,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G32" activeCellId="0" pane="topLeft" sqref="G32"/>
+      <selection activeCell="K11" activeCellId="0" pane="topLeft" sqref="K10:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -5933,9 +5997,15 @@
       <c r="E16" s="7" t="n">
         <v>0.83</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="F16" s="7" t="n">
+        <v>0.7405</v>
+      </c>
+      <c r="G16" s="7" t="n">
+        <v>0.69</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <v>0.765</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="4" t="s">
@@ -6295,9 +6365,15 @@
       <c r="E34" s="7" t="n">
         <v>0.825</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
+      <c r="F34" s="7" t="n">
+        <v>0.7515</v>
+      </c>
+      <c r="G34" s="7" t="n">
+        <v>0.685</v>
+      </c>
+      <c r="H34" s="7" t="n">
+        <v>0.825</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>